<commit_message>
Präsentationh zu Ergebnissen der ersten Woche
</commit_message>
<xml_diff>
--- a/Bufdi_Tagebuch.xlsx
+++ b/Bufdi_Tagebuch.xlsx
@@ -68,10 +68,10 @@
     <t>Lese-/ Recherchaufgabe "ethical dilemma in research"; Vorbereitung Präsentation; Organisation Dateien</t>
   </si>
   <si>
-    <t>Auswertung research, Präsentation der Wochenergebnisse, Einrichtung Github mit Git Bash</t>
+    <t>Github, Git Bash; PyCharm</t>
   </si>
   <si>
-    <t>Github, Git Bash</t>
+    <t xml:space="preserve">Auswertung Research; Präsentation der Wochenergebnisse; Einrichtung Github mit Git Bash; Einführung Open_Modex </t>
   </si>
 </sst>
 </file>
@@ -515,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:X368"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,7 +694,7 @@
         <v>44414</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="9"/>
@@ -714,7 +714,7 @@
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="V10" s="11"/>
       <c r="W10" s="11"/>

</xml_diff>

<commit_message>
Woche 19 bis 30
</commit_message>
<xml_diff>
--- a/Bufdi_Tagebuch.xlsx
+++ b/Bufdi_Tagebuch.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="156">
   <si>
     <t>Bufdi Tagebuch</t>
   </si>
@@ -401,6 +401,157 @@
   </si>
   <si>
     <t>Weihnachtsfeier Nachbereitung, Mails, Validierungsdaten Haushaltsstromedarfszeitreihen</t>
+  </si>
+  <si>
+    <t>Lebensläufe auf neues Format aktualisieren, Einkauf von Schnelltests für das Büro</t>
+  </si>
+  <si>
+    <t>Validierungsdaten eGo^n, Unterstützung Abschlussbericht UMAS</t>
+  </si>
+  <si>
+    <t>Christians Geschenk vorbereiten und basteln, Termine vereinbaren, Unterstützung für Sustainable Transport Workshop</t>
+  </si>
+  <si>
+    <t>OEP: Model Factsheets ergänzen, Locationanfrage RLI Klausur, Endredaktion TVB EmpowerPlan</t>
+  </si>
+  <si>
+    <t>Admin-Vertretung: Betreuung Empfangsbüro, Post, Paketannahme, Büroräume checken; Endredaktion TVB EmpowerPlan</t>
+  </si>
+  <si>
+    <t>Auswertung Menti Umfrage Sommerparty, MA-Runde, Paket abholen, Absprache OEP: Model Factsheets auf neusten Stand bringen</t>
+  </si>
+  <si>
+    <t>Test Nextcloud, OEP: Modelfactsheets ergänzen, Internetausfall</t>
+  </si>
+  <si>
+    <t>Design, Erstellung Jubiläumskarten</t>
+  </si>
+  <si>
+    <t>Meeting zu Jahresplanung Events, Location Suche für Sommerparty und Klausur, Orga-Tätigkeiten im Büro</t>
+  </si>
+  <si>
+    <t>GVB StadtLandEnergie: xls-Auszüge + Tabellen bearbeiten &amp; einfügen, Struckturplan erstellen, Projektmeeting</t>
+  </si>
+  <si>
+    <t>Teammeeting; GVB StadtLandEnergie: xls-Auszüge erneuern, weitere jpgs einfügen, Struckturplan überarbeiten</t>
+  </si>
+  <si>
+    <t>GVB StadtLandEnergie finallisieren: jpgs einfügen, Korrektur lesen, Zeilenumbrüche und weitere Formatierung, letztes Meeting zur Absprache</t>
+  </si>
+  <si>
+    <t>Nextcloud testen, Überarbeitung Wikipedia Artikel eGo Tools</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GVB StadtLandEnergie: Meeting zur Absprache, Formatierungsaufgaben </t>
+  </si>
+  <si>
+    <t>Feedbackgespräch, Projektreport einschl. Vor- und Nachbereitung, 12 Jahre RLI Jubiläum, GVB StadtLandEnergie</t>
+  </si>
+  <si>
+    <t>GVB StadtLandEnergie: Tabellen formatieren, TODOs spezifizieren, Projektmeeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Teammeeting, Zwischenstand Umfrage Sommerparty auswerten, GVB StadtLandEnergie bearbeiten </t>
+  </si>
+  <si>
+    <t>StadtLandEnergie Projektmeeting, Arbeit an GVB, Meilensteine aktualisieren/formatieren</t>
+  </si>
+  <si>
+    <t>Boards sichern, Vorbereitung MA-Runde, Team Orga</t>
+  </si>
+  <si>
+    <t>Teammeeting Protokoll im Redmine ablegen, GVB StadtLandEnergie Endredaktion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Christians Abschiedsgeschenk basteln; Orga Abschiedsfeier: Einkauf, Set up; Abschiedsevent </t>
+  </si>
+  <si>
+    <t>Boards sichern, Unterstützung bei Admin Orga</t>
+  </si>
+  <si>
+    <t>Recherche eGo^n Wärmepumpen</t>
+  </si>
+  <si>
+    <t>Absprache mit Sarah zu Erstellung der GVB StadtLandEnergie, Erstellung von Latex Layout für GVB</t>
+  </si>
+  <si>
+    <t>Text für RLI Webseite über das WWF Dasboard erstellen, Boards sichern, SLE Texte aus easyonline übersetzen</t>
+  </si>
+  <si>
+    <t>Erstellung von Latex Layout für GVB, Teammeeting, Covid Impfung</t>
+  </si>
+  <si>
+    <t>Teammeeting Protokll, GVB StadtLandEnergie: Vorlage Reisekostentabelle an Vorlage aus PtJ Schreiben anpassen, SLE Kick-Off, Austausch Wärmepumpen mit OG</t>
+  </si>
+  <si>
+    <t>Serientermin Zoom für Projektmeetings SLE, gantt Diagramm erstellen, SLE Projektmeeting, Feedbackgespräch</t>
+  </si>
+  <si>
+    <t>Kommunikation mit Projektpartnern SLE, Boards sichern, Aufgaben in der GVB StadtLandEnergie</t>
+  </si>
+  <si>
+    <t>GVB StadtLandEnergie: TODOs abarbeiten, Referenzen einfügen, Crashkurs Mentimeter für Marius</t>
+  </si>
+  <si>
+    <t>RLI-interne Absprache zu SLE, Projektreport inklusive Vor- und Nachbereitung, Webinar der TU zu nachhaltigen Studiengängen</t>
+  </si>
+  <si>
+    <t>OEP: Model Factsheets ergänzen, Team-Meeting, OG Bufdi Führung, Orga RLI Klausur, Feedbackgespräch, Tagebuch überarbeiten/aktualisieren</t>
+  </si>
+  <si>
+    <t>Projektmeeting SLE, Texte verfassen für GVB</t>
+  </si>
+  <si>
+    <t>Boards sichern, Arbeit mit den Kalkulationstabellen für StadtLandEnergie</t>
+  </si>
+  <si>
+    <t>MA-Runde, Erstellung Menti Umfrage: Sommer-Weihnachtsfeier, erste Location Suche</t>
+  </si>
+  <si>
+    <t>Teammeeting, Projektmeeting SLE, Doku Teamtage finalisieren,  Absprache Wikipedia eGo-Tools mit Anya</t>
+  </si>
+  <si>
+    <t>Teammeeting Protokoll ins Redmine, Erstellung der Texte für Wikipedia</t>
+  </si>
+  <si>
+    <t>Projektmeeting SLE, Boards sichern, Aufgaben für GVB StadtLandEnergie</t>
+  </si>
+  <si>
+    <t>Seminar "Grüne Berufe"</t>
+  </si>
+  <si>
+    <t>Seminar "Weltbewusst"</t>
+  </si>
+  <si>
+    <t>Projektmeeting SLE, GVB StadtLandEnergie: Meilenstein Liste überarbeiten, Thursday Updates on Energy Modeling</t>
+  </si>
+  <si>
+    <t>Boards sichern, Erstellung Wikipedia Artikel eGo Tools</t>
+  </si>
+  <si>
+    <t>Organisation meines Daten-/Ordnermanagements, abschließende organisatorische Tätigkeiten</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>GVB StadtLandEnergie,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> krank</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -869,15 +1020,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Y368"/>
+  <dimension ref="A3:Y368"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C371" sqref="C371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="2:25" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
@@ -888,7 +1039,7 @@
       </c>
       <c r="G3" s="4"/>
     </row>
-    <row r="5" spans="2:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -922,7 +1073,10 @@
       <c r="X5" s="1"/>
       <c r="Y5" s="1"/>
     </row>
-    <row r="6" spans="2:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
       <c r="B6" s="8">
         <v>44410</v>
       </c>
@@ -954,7 +1108,7 @@
       <c r="X6" s="11"/>
       <c r="Y6" s="11"/>
     </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>44411</v>
       </c>
@@ -986,7 +1140,7 @@
       <c r="X7" s="11"/>
       <c r="Y7" s="11"/>
     </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>44412</v>
       </c>
@@ -1020,7 +1174,7 @@
       <c r="X8" s="11"/>
       <c r="Y8" s="11"/>
     </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>44413</v>
       </c>
@@ -1052,7 +1206,7 @@
       <c r="X9" s="11"/>
       <c r="Y9" s="11"/>
     </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>44414</v>
       </c>
@@ -1084,7 +1238,7 @@
       <c r="X10" s="11"/>
       <c r="Y10" s="11"/>
     </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="12">
         <v>44415</v>
       </c>
@@ -1112,7 +1266,7 @@
       <c r="X11" s="15"/>
       <c r="Y11" s="15"/>
     </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="12">
         <v>44416</v>
       </c>
@@ -1140,7 +1294,10 @@
       <c r="X12" s="15"/>
       <c r="Y12" s="15"/>
     </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2</v>
+      </c>
       <c r="B13" s="8">
         <v>44417</v>
       </c>
@@ -1174,7 +1331,7 @@
       <c r="X13" s="11"/>
       <c r="Y13" s="11"/>
     </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>44418</v>
       </c>
@@ -1206,7 +1363,7 @@
       <c r="X14" s="11"/>
       <c r="Y14" s="11"/>
     </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
         <v>44419</v>
       </c>
@@ -1236,7 +1393,7 @@
       <c r="X15" s="11"/>
       <c r="Y15" s="11"/>
     </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>44420</v>
       </c>
@@ -1266,7 +1423,7 @@
       <c r="X16" s="11"/>
       <c r="Y16" s="11"/>
     </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>44421</v>
       </c>
@@ -1298,7 +1455,7 @@
       <c r="X17" s="11"/>
       <c r="Y17" s="11"/>
     </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B18" s="12">
         <v>44422</v>
       </c>
@@ -1326,7 +1483,7 @@
       <c r="X18" s="15"/>
       <c r="Y18" s="15"/>
     </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B19" s="12">
         <v>44423</v>
       </c>
@@ -1354,7 +1511,10 @@
       <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
     </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
       <c r="B20" s="8">
         <v>44424</v>
       </c>
@@ -1388,7 +1548,7 @@
       <c r="X20" s="11"/>
       <c r="Y20" s="11"/>
     </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
         <v>44425</v>
       </c>
@@ -1418,7 +1578,7 @@
       <c r="X21" s="11"/>
       <c r="Y21" s="11"/>
     </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>44426</v>
       </c>
@@ -1448,7 +1608,7 @@
       <c r="X22" s="11"/>
       <c r="Y22" s="11"/>
     </row>
-    <row r="23" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>44427</v>
       </c>
@@ -1478,7 +1638,7 @@
       <c r="X23" s="11"/>
       <c r="Y23" s="11"/>
     </row>
-    <row r="24" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
         <v>44428</v>
       </c>
@@ -1510,7 +1670,7 @@
       <c r="X24" s="11"/>
       <c r="Y24" s="11"/>
     </row>
-    <row r="25" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B25" s="12">
         <v>44429</v>
       </c>
@@ -1538,7 +1698,7 @@
       <c r="X25" s="15"/>
       <c r="Y25" s="15"/>
     </row>
-    <row r="26" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B26" s="12">
         <v>44430</v>
       </c>
@@ -1566,7 +1726,10 @@
       <c r="X26" s="15"/>
       <c r="Y26" s="15"/>
     </row>
-    <row r="27" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
       <c r="B27" s="8">
         <v>44431</v>
       </c>
@@ -1598,7 +1761,7 @@
       <c r="X27" s="11"/>
       <c r="Y27" s="11"/>
     </row>
-    <row r="28" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
         <v>44432</v>
       </c>
@@ -1628,7 +1791,7 @@
       <c r="X28" s="11"/>
       <c r="Y28" s="11"/>
     </row>
-    <row r="29" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
         <v>44433</v>
       </c>
@@ -1658,7 +1821,7 @@
       <c r="X29" s="11"/>
       <c r="Y29" s="11"/>
     </row>
-    <row r="30" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
         <v>44434</v>
       </c>
@@ -1688,7 +1851,7 @@
       <c r="X30" s="11"/>
       <c r="Y30" s="11"/>
     </row>
-    <row r="31" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
         <v>44435</v>
       </c>
@@ -1718,7 +1881,7 @@
       <c r="X31" s="11"/>
       <c r="Y31" s="11"/>
     </row>
-    <row r="32" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B32" s="12">
         <v>44436</v>
       </c>
@@ -1746,7 +1909,7 @@
       <c r="X32" s="15"/>
       <c r="Y32" s="15"/>
     </row>
-    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B33" s="12">
         <v>44437</v>
       </c>
@@ -1774,7 +1937,10 @@
       <c r="X33" s="15"/>
       <c r="Y33" s="15"/>
     </row>
-    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>5</v>
+      </c>
       <c r="B34" s="8">
         <v>44438</v>
       </c>
@@ -1808,7 +1974,7 @@
       <c r="X34" s="11"/>
       <c r="Y34" s="11"/>
     </row>
-    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
         <v>44439</v>
       </c>
@@ -1838,7 +2004,7 @@
       <c r="X35" s="11"/>
       <c r="Y35" s="11"/>
     </row>
-    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
         <v>44440</v>
       </c>
@@ -1868,7 +2034,7 @@
       <c r="X36" s="11"/>
       <c r="Y36" s="11"/>
     </row>
-    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
         <v>44441</v>
       </c>
@@ -1898,7 +2064,7 @@
       <c r="X37" s="11"/>
       <c r="Y37" s="11"/>
     </row>
-    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B38" s="8">
         <v>44442</v>
       </c>
@@ -1928,7 +2094,7 @@
       <c r="X38" s="11"/>
       <c r="Y38" s="11"/>
     </row>
-    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B39" s="12">
         <v>44443</v>
       </c>
@@ -1956,7 +2122,7 @@
       <c r="X39" s="15"/>
       <c r="Y39" s="15"/>
     </row>
-    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B40" s="12">
         <v>44444</v>
       </c>
@@ -1984,7 +2150,10 @@
       <c r="X40" s="15"/>
       <c r="Y40" s="15"/>
     </row>
-    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
       <c r="B41" s="8">
         <v>44445</v>
       </c>
@@ -2016,7 +2185,7 @@
       <c r="X41" s="11"/>
       <c r="Y41" s="11"/>
     </row>
-    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B42" s="8">
         <v>44446</v>
       </c>
@@ -2046,7 +2215,7 @@
       <c r="X42" s="11"/>
       <c r="Y42" s="11"/>
     </row>
-    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B43" s="8">
         <v>44447</v>
       </c>
@@ -2076,7 +2245,7 @@
       <c r="X43" s="11"/>
       <c r="Y43" s="11"/>
     </row>
-    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B44" s="8">
         <v>44448</v>
       </c>
@@ -2106,7 +2275,7 @@
       <c r="X44" s="11"/>
       <c r="Y44" s="11"/>
     </row>
-    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B45" s="8">
         <v>44449</v>
       </c>
@@ -2134,7 +2303,7 @@
       <c r="X45" s="11"/>
       <c r="Y45" s="11"/>
     </row>
-    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B46" s="12">
         <v>44450</v>
       </c>
@@ -2162,7 +2331,7 @@
       <c r="X46" s="15"/>
       <c r="Y46" s="15"/>
     </row>
-    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B47" s="12">
         <v>44451</v>
       </c>
@@ -2190,7 +2359,10 @@
       <c r="X47" s="15"/>
       <c r="Y47" s="15"/>
     </row>
-    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>7</v>
+      </c>
       <c r="B48" s="8">
         <v>44452</v>
       </c>
@@ -2222,7 +2394,7 @@
       <c r="X48" s="11"/>
       <c r="Y48" s="11"/>
     </row>
-    <row r="49" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B49" s="8">
         <v>44453</v>
       </c>
@@ -2252,7 +2424,7 @@
       <c r="X49" s="11"/>
       <c r="Y49" s="11"/>
     </row>
-    <row r="50" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B50" s="8">
         <v>44454</v>
       </c>
@@ -2284,7 +2456,7 @@
       <c r="X50" s="11"/>
       <c r="Y50" s="11"/>
     </row>
-    <row r="51" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B51" s="8">
         <v>44455</v>
       </c>
@@ -2314,7 +2486,7 @@
       <c r="X51" s="11"/>
       <c r="Y51" s="11"/>
     </row>
-    <row r="52" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B52" s="8">
         <v>44456</v>
       </c>
@@ -2344,7 +2516,7 @@
       <c r="X52" s="11"/>
       <c r="Y52" s="11"/>
     </row>
-    <row r="53" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B53" s="12">
         <v>44457</v>
       </c>
@@ -2372,7 +2544,7 @@
       <c r="X53" s="15"/>
       <c r="Y53" s="15"/>
     </row>
-    <row r="54" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B54" s="12">
         <v>44458</v>
       </c>
@@ -2400,7 +2572,10 @@
       <c r="X54" s="15"/>
       <c r="Y54" s="15"/>
     </row>
-    <row r="55" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>8</v>
+      </c>
       <c r="B55" s="8">
         <v>44459</v>
       </c>
@@ -2430,7 +2605,7 @@
       <c r="X55" s="11"/>
       <c r="Y55" s="11"/>
     </row>
-    <row r="56" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B56" s="8">
         <v>44460</v>
       </c>
@@ -2460,7 +2635,7 @@
       <c r="X56" s="11"/>
       <c r="Y56" s="11"/>
     </row>
-    <row r="57" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B57" s="8">
         <v>44461</v>
       </c>
@@ -2490,7 +2665,7 @@
       <c r="X57" s="11"/>
       <c r="Y57" s="11"/>
     </row>
-    <row r="58" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B58" s="8">
         <v>44462</v>
       </c>
@@ -2520,7 +2695,7 @@
       <c r="X58" s="11"/>
       <c r="Y58" s="11"/>
     </row>
-    <row r="59" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B59" s="8">
         <v>44463</v>
       </c>
@@ -2550,7 +2725,7 @@
       <c r="X59" s="11"/>
       <c r="Y59" s="11"/>
     </row>
-    <row r="60" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B60" s="12">
         <v>44464</v>
       </c>
@@ -2578,7 +2753,7 @@
       <c r="X60" s="15"/>
       <c r="Y60" s="15"/>
     </row>
-    <row r="61" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B61" s="12">
         <v>44465</v>
       </c>
@@ -2606,7 +2781,10 @@
       <c r="X61" s="15"/>
       <c r="Y61" s="15"/>
     </row>
-    <row r="62" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>9</v>
+      </c>
       <c r="B62" s="8">
         <v>44466</v>
       </c>
@@ -2636,7 +2814,7 @@
       <c r="X62" s="11"/>
       <c r="Y62" s="11"/>
     </row>
-    <row r="63" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B63" s="8">
         <v>44467</v>
       </c>
@@ -2666,7 +2844,7 @@
       <c r="X63" s="11"/>
       <c r="Y63" s="11"/>
     </row>
-    <row r="64" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B64" s="8">
         <v>44468</v>
       </c>
@@ -2696,7 +2874,7 @@
       <c r="X64" s="11"/>
       <c r="Y64" s="11"/>
     </row>
-    <row r="65" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B65" s="8">
         <v>44469</v>
       </c>
@@ -2726,7 +2904,7 @@
       <c r="X65" s="11"/>
       <c r="Y65" s="11"/>
     </row>
-    <row r="66" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B66" s="8">
         <v>44470</v>
       </c>
@@ -2756,7 +2934,7 @@
       <c r="X66" s="11"/>
       <c r="Y66" s="11"/>
     </row>
-    <row r="67" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B67" s="12">
         <v>44471</v>
       </c>
@@ -2784,7 +2962,7 @@
       <c r="X67" s="15"/>
       <c r="Y67" s="15"/>
     </row>
-    <row r="68" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B68" s="12">
         <v>44472</v>
       </c>
@@ -2812,7 +2990,10 @@
       <c r="X68" s="15"/>
       <c r="Y68" s="15"/>
     </row>
-    <row r="69" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>10</v>
+      </c>
       <c r="B69" s="8">
         <v>44473</v>
       </c>
@@ -2842,7 +3023,7 @@
       <c r="X69" s="11"/>
       <c r="Y69" s="11"/>
     </row>
-    <row r="70" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B70" s="8">
         <v>44474</v>
       </c>
@@ -2874,7 +3055,7 @@
       <c r="X70" s="11"/>
       <c r="Y70" s="11"/>
     </row>
-    <row r="71" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B71" s="8">
         <v>44475</v>
       </c>
@@ -2904,7 +3085,7 @@
       <c r="X71" s="11"/>
       <c r="Y71" s="11"/>
     </row>
-    <row r="72" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B72" s="8">
         <v>44476</v>
       </c>
@@ -2934,7 +3115,7 @@
       <c r="X72" s="11"/>
       <c r="Y72" s="11"/>
     </row>
-    <row r="73" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B73" s="8">
         <v>44477</v>
       </c>
@@ -2964,7 +3145,7 @@
       <c r="X73" s="11"/>
       <c r="Y73" s="11"/>
     </row>
-    <row r="74" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B74" s="12">
         <v>44478</v>
       </c>
@@ -2992,7 +3173,7 @@
       <c r="X74" s="15"/>
       <c r="Y74" s="15"/>
     </row>
-    <row r="75" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B75" s="12">
         <v>44479</v>
       </c>
@@ -3020,7 +3201,10 @@
       <c r="X75" s="15"/>
       <c r="Y75" s="15"/>
     </row>
-    <row r="76" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>11</v>
+      </c>
       <c r="B76" s="8">
         <v>44480</v>
       </c>
@@ -3050,7 +3234,7 @@
       <c r="X76" s="11"/>
       <c r="Y76" s="11"/>
     </row>
-    <row r="77" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B77" s="8">
         <v>44481</v>
       </c>
@@ -3082,7 +3266,7 @@
       <c r="X77" s="11"/>
       <c r="Y77" s="11"/>
     </row>
-    <row r="78" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B78" s="8">
         <v>44482</v>
       </c>
@@ -3114,7 +3298,7 @@
       <c r="X78" s="11"/>
       <c r="Y78" s="11"/>
     </row>
-    <row r="79" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B79" s="8">
         <v>44483</v>
       </c>
@@ -3144,7 +3328,7 @@
       <c r="X79" s="11"/>
       <c r="Y79" s="11"/>
     </row>
-    <row r="80" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B80" s="8">
         <v>44484</v>
       </c>
@@ -3174,7 +3358,7 @@
       <c r="X80" s="11"/>
       <c r="Y80" s="11"/>
     </row>
-    <row r="81" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B81" s="12">
         <v>44485</v>
       </c>
@@ -3202,7 +3386,7 @@
       <c r="X81" s="15"/>
       <c r="Y81" s="15"/>
     </row>
-    <row r="82" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B82" s="12">
         <v>44486</v>
       </c>
@@ -3230,7 +3414,10 @@
       <c r="X82" s="15"/>
       <c r="Y82" s="15"/>
     </row>
-    <row r="83" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>12</v>
+      </c>
       <c r="B83" s="8">
         <v>44487</v>
       </c>
@@ -3260,7 +3447,7 @@
       <c r="X83" s="11"/>
       <c r="Y83" s="11"/>
     </row>
-    <row r="84" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B84" s="8">
         <v>44488</v>
       </c>
@@ -3290,7 +3477,7 @@
       <c r="X84" s="11"/>
       <c r="Y84" s="11"/>
     </row>
-    <row r="85" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B85" s="8">
         <v>44489</v>
       </c>
@@ -3320,7 +3507,7 @@
       <c r="X85" s="11"/>
       <c r="Y85" s="11"/>
     </row>
-    <row r="86" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B86" s="8">
         <v>44490</v>
       </c>
@@ -3350,7 +3537,7 @@
       <c r="X86" s="11"/>
       <c r="Y86" s="11"/>
     </row>
-    <row r="87" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B87" s="8">
         <v>44491</v>
       </c>
@@ -3380,7 +3567,7 @@
       <c r="X87" s="11"/>
       <c r="Y87" s="11"/>
     </row>
-    <row r="88" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B88" s="12">
         <v>44492</v>
       </c>
@@ -3408,7 +3595,7 @@
       <c r="X88" s="15"/>
       <c r="Y88" s="15"/>
     </row>
-    <row r="89" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B89" s="12">
         <v>44493</v>
       </c>
@@ -3436,7 +3623,10 @@
       <c r="X89" s="15"/>
       <c r="Y89" s="15"/>
     </row>
-    <row r="90" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>13</v>
+      </c>
       <c r="B90" s="8">
         <v>44494</v>
       </c>
@@ -3466,7 +3656,7 @@
       <c r="X90" s="11"/>
       <c r="Y90" s="11"/>
     </row>
-    <row r="91" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B91" s="8">
         <v>44495</v>
       </c>
@@ -3496,7 +3686,7 @@
       <c r="X91" s="11"/>
       <c r="Y91" s="11"/>
     </row>
-    <row r="92" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B92" s="8">
         <v>44496</v>
       </c>
@@ -3528,7 +3718,7 @@
       <c r="X92" s="11"/>
       <c r="Y92" s="11"/>
     </row>
-    <row r="93" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B93" s="8">
         <v>44497</v>
       </c>
@@ -3558,7 +3748,7 @@
       <c r="X93" s="11"/>
       <c r="Y93" s="11"/>
     </row>
-    <row r="94" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B94" s="8">
         <v>44498</v>
       </c>
@@ -3588,7 +3778,7 @@
       <c r="X94" s="11"/>
       <c r="Y94" s="11"/>
     </row>
-    <row r="95" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B95" s="12">
         <v>44499</v>
       </c>
@@ -3616,7 +3806,7 @@
       <c r="X95" s="15"/>
       <c r="Y95" s="15"/>
     </row>
-    <row r="96" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B96" s="12">
         <v>44500</v>
       </c>
@@ -3644,7 +3834,10 @@
       <c r="X96" s="15"/>
       <c r="Y96" s="15"/>
     </row>
-    <row r="97" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>14</v>
+      </c>
       <c r="B97" s="8">
         <v>44501</v>
       </c>
@@ -3676,7 +3869,7 @@
       <c r="X97" s="11"/>
       <c r="Y97" s="11"/>
     </row>
-    <row r="98" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B98" s="8">
         <v>44502</v>
       </c>
@@ -3708,7 +3901,7 @@
       <c r="X98" s="11"/>
       <c r="Y98" s="11"/>
     </row>
-    <row r="99" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B99" s="8">
         <v>44503</v>
       </c>
@@ -3738,7 +3931,7 @@
       <c r="X99" s="11"/>
       <c r="Y99" s="11"/>
     </row>
-    <row r="100" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B100" s="8">
         <v>44504</v>
       </c>
@@ -3770,7 +3963,7 @@
       <c r="X100" s="11"/>
       <c r="Y100" s="11"/>
     </row>
-    <row r="101" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B101" s="8">
         <v>44505</v>
       </c>
@@ -3800,7 +3993,7 @@
       <c r="X101" s="11"/>
       <c r="Y101" s="11"/>
     </row>
-    <row r="102" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B102" s="12">
         <v>44506</v>
       </c>
@@ -3828,7 +4021,7 @@
       <c r="X102" s="15"/>
       <c r="Y102" s="15"/>
     </row>
-    <row r="103" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B103" s="12">
         <v>44507</v>
       </c>
@@ -3856,7 +4049,10 @@
       <c r="X103" s="15"/>
       <c r="Y103" s="15"/>
     </row>
-    <row r="104" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>15</v>
+      </c>
       <c r="B104" s="8">
         <v>44508</v>
       </c>
@@ -3886,7 +4082,7 @@
       <c r="X104" s="11"/>
       <c r="Y104" s="11"/>
     </row>
-    <row r="105" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B105" s="8">
         <v>44509</v>
       </c>
@@ -3916,7 +4112,7 @@
       <c r="X105" s="11"/>
       <c r="Y105" s="11"/>
     </row>
-    <row r="106" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B106" s="8">
         <v>44510</v>
       </c>
@@ -3948,7 +4144,7 @@
       <c r="X106" s="11"/>
       <c r="Y106" s="11"/>
     </row>
-    <row r="107" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B107" s="8">
         <v>44511</v>
       </c>
@@ -3978,7 +4174,7 @@
       <c r="X107" s="11"/>
       <c r="Y107" s="11"/>
     </row>
-    <row r="108" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B108" s="8">
         <v>44512</v>
       </c>
@@ -4008,7 +4204,7 @@
       <c r="X108" s="11"/>
       <c r="Y108" s="11"/>
     </row>
-    <row r="109" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B109" s="12">
         <v>44513</v>
       </c>
@@ -4036,7 +4232,7 @@
       <c r="X109" s="15"/>
       <c r="Y109" s="15"/>
     </row>
-    <row r="110" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B110" s="12">
         <v>44514</v>
       </c>
@@ -4064,7 +4260,10 @@
       <c r="X110" s="15"/>
       <c r="Y110" s="15"/>
     </row>
-    <row r="111" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A111">
+        <v>16</v>
+      </c>
       <c r="B111" s="8">
         <v>44515</v>
       </c>
@@ -4094,7 +4293,7 @@
       <c r="X111" s="11"/>
       <c r="Y111" s="11"/>
     </row>
-    <row r="112" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B112" s="8">
         <v>44516</v>
       </c>
@@ -4124,7 +4323,7 @@
       <c r="X112" s="11"/>
       <c r="Y112" s="11"/>
     </row>
-    <row r="113" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B113" s="8">
         <v>44517</v>
       </c>
@@ -4154,7 +4353,7 @@
       <c r="X113" s="11"/>
       <c r="Y113" s="11"/>
     </row>
-    <row r="114" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B114" s="8">
         <v>44518</v>
       </c>
@@ -4184,7 +4383,7 @@
       <c r="X114" s="11"/>
       <c r="Y114" s="11"/>
     </row>
-    <row r="115" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B115" s="8">
         <v>44519</v>
       </c>
@@ -4214,7 +4413,7 @@
       <c r="X115" s="11"/>
       <c r="Y115" s="11"/>
     </row>
-    <row r="116" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B116" s="12">
         <v>44520</v>
       </c>
@@ -4242,7 +4441,7 @@
       <c r="X116" s="15"/>
       <c r="Y116" s="15"/>
     </row>
-    <row r="117" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B117" s="12">
         <v>44521</v>
       </c>
@@ -4270,7 +4469,10 @@
       <c r="X117" s="15"/>
       <c r="Y117" s="15"/>
     </row>
-    <row r="118" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>17</v>
+      </c>
       <c r="B118" s="8">
         <v>44522</v>
       </c>
@@ -4300,7 +4502,7 @@
       <c r="X118" s="11"/>
       <c r="Y118" s="11"/>
     </row>
-    <row r="119" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B119" s="8">
         <v>44523</v>
       </c>
@@ -4330,7 +4532,7 @@
       <c r="X119" s="11"/>
       <c r="Y119" s="11"/>
     </row>
-    <row r="120" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B120" s="8">
         <v>44524</v>
       </c>
@@ -4360,7 +4562,7 @@
       <c r="X120" s="11"/>
       <c r="Y120" s="11"/>
     </row>
-    <row r="121" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B121" s="8">
         <v>44525</v>
       </c>
@@ -4390,7 +4592,7 @@
       <c r="X121" s="11"/>
       <c r="Y121" s="11"/>
     </row>
-    <row r="122" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B122" s="8">
         <v>44526</v>
       </c>
@@ -4420,7 +4622,7 @@
       <c r="X122" s="11"/>
       <c r="Y122" s="11"/>
     </row>
-    <row r="123" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B123" s="12">
         <v>44527</v>
       </c>
@@ -4448,7 +4650,7 @@
       <c r="X123" s="15"/>
       <c r="Y123" s="15"/>
     </row>
-    <row r="124" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B124" s="12">
         <v>44528</v>
       </c>
@@ -4476,7 +4678,10 @@
       <c r="X124" s="15"/>
       <c r="Y124" s="15"/>
     </row>
-    <row r="125" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>18</v>
+      </c>
       <c r="B125" s="8">
         <v>44529</v>
       </c>
@@ -4506,7 +4711,7 @@
       <c r="X125" s="11"/>
       <c r="Y125" s="11"/>
     </row>
-    <row r="126" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B126" s="8">
         <v>44530</v>
       </c>
@@ -4536,7 +4741,7 @@
       <c r="X126" s="11"/>
       <c r="Y126" s="11"/>
     </row>
-    <row r="127" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B127" s="8">
         <v>44531</v>
       </c>
@@ -4566,7 +4771,7 @@
       <c r="X127" s="11"/>
       <c r="Y127" s="11"/>
     </row>
-    <row r="128" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B128" s="8">
         <v>44532</v>
       </c>
@@ -4596,7 +4801,7 @@
       <c r="X128" s="11"/>
       <c r="Y128" s="11"/>
     </row>
-    <row r="129" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B129" s="8">
         <v>44533</v>
       </c>
@@ -4626,7 +4831,7 @@
       <c r="X129" s="11"/>
       <c r="Y129" s="11"/>
     </row>
-    <row r="130" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B130" s="12">
         <v>44534</v>
       </c>
@@ -4654,7 +4859,7 @@
       <c r="X130" s="15"/>
       <c r="Y130" s="15"/>
     </row>
-    <row r="131" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B131" s="12">
         <v>44535</v>
       </c>
@@ -4682,7 +4887,10 @@
       <c r="X131" s="15"/>
       <c r="Y131" s="15"/>
     </row>
-    <row r="132" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>19</v>
+      </c>
       <c r="B132" s="8">
         <v>44536</v>
       </c>
@@ -4712,7 +4920,7 @@
       <c r="X132" s="11"/>
       <c r="Y132" s="11"/>
     </row>
-    <row r="133" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B133" s="8">
         <v>44537</v>
       </c>
@@ -4742,7 +4950,7 @@
       <c r="X133" s="11"/>
       <c r="Y133" s="11"/>
     </row>
-    <row r="134" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B134" s="8">
         <v>44538</v>
       </c>
@@ -4772,7 +4980,7 @@
       <c r="X134" s="11"/>
       <c r="Y134" s="11"/>
     </row>
-    <row r="135" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B135" s="8">
         <v>44539</v>
       </c>
@@ -4802,7 +5010,7 @@
       <c r="X135" s="11"/>
       <c r="Y135" s="11"/>
     </row>
-    <row r="136" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B136" s="8">
         <v>44540</v>
       </c>
@@ -4832,7 +5040,7 @@
       <c r="X136" s="11"/>
       <c r="Y136" s="11"/>
     </row>
-    <row r="137" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B137" s="12">
         <v>44541</v>
       </c>
@@ -4860,7 +5068,7 @@
       <c r="X137" s="15"/>
       <c r="Y137" s="15"/>
     </row>
-    <row r="138" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B138" s="12">
         <v>44542</v>
       </c>
@@ -4888,11 +5096,16 @@
       <c r="X138" s="15"/>
       <c r="Y138" s="15"/>
     </row>
-    <row r="139" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>20</v>
+      </c>
       <c r="B139" s="8">
         <v>44543</v>
       </c>
-      <c r="C139" s="9"/>
+      <c r="C139" s="16" t="s">
+        <v>113</v>
+      </c>
       <c r="D139" s="9"/>
       <c r="E139" s="9"/>
       <c r="F139" s="9"/>
@@ -4916,11 +5129,13 @@
       <c r="X139" s="11"/>
       <c r="Y139" s="11"/>
     </row>
-    <row r="140" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B140" s="8">
         <v>44544</v>
       </c>
-      <c r="C140" s="9"/>
+      <c r="C140" s="16" t="s">
+        <v>114</v>
+      </c>
       <c r="D140" s="9"/>
       <c r="E140" s="9"/>
       <c r="F140" s="9"/>
@@ -4944,11 +5159,13 @@
       <c r="X140" s="11"/>
       <c r="Y140" s="11"/>
     </row>
-    <row r="141" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B141" s="8">
         <v>44545</v>
       </c>
-      <c r="C141" s="9"/>
+      <c r="C141" s="16" t="s">
+        <v>112</v>
+      </c>
       <c r="D141" s="9"/>
       <c r="E141" s="9"/>
       <c r="F141" s="9"/>
@@ -4972,11 +5189,13 @@
       <c r="X141" s="11"/>
       <c r="Y141" s="11"/>
     </row>
-    <row r="142" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B142" s="8">
         <v>44546</v>
       </c>
-      <c r="C142" s="9"/>
+      <c r="C142" s="16" t="s">
+        <v>132</v>
+      </c>
       <c r="D142" s="9"/>
       <c r="E142" s="9"/>
       <c r="F142" s="9"/>
@@ -5000,11 +5219,13 @@
       <c r="X142" s="11"/>
       <c r="Y142" s="11"/>
     </row>
-    <row r="143" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B143" s="8">
         <v>44547</v>
       </c>
-      <c r="C143" s="9"/>
+      <c r="C143" s="16" t="s">
+        <v>133</v>
+      </c>
       <c r="D143" s="9"/>
       <c r="E143" s="9"/>
       <c r="F143" s="9"/>
@@ -5028,7 +5249,7 @@
       <c r="X143" s="11"/>
       <c r="Y143" s="11"/>
     </row>
-    <row r="144" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B144" s="12">
         <v>44548</v>
       </c>
@@ -5056,7 +5277,7 @@
       <c r="X144" s="15"/>
       <c r="Y144" s="15"/>
     </row>
-    <row r="145" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B145" s="12">
         <v>44549</v>
       </c>
@@ -5084,11 +5305,16 @@
       <c r="X145" s="15"/>
       <c r="Y145" s="15"/>
     </row>
-    <row r="146" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>21</v>
+      </c>
       <c r="B146" s="8">
         <v>44550</v>
       </c>
-      <c r="C146" s="9"/>
+      <c r="C146" s="16" t="s">
+        <v>134</v>
+      </c>
       <c r="D146" s="9"/>
       <c r="E146" s="9"/>
       <c r="F146" s="9"/>
@@ -5112,11 +5338,13 @@
       <c r="X146" s="11"/>
       <c r="Y146" s="11"/>
     </row>
-    <row r="147" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B147" s="8">
         <v>44551</v>
       </c>
-      <c r="C147" s="9"/>
+      <c r="C147" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="D147" s="9"/>
       <c r="E147" s="9"/>
       <c r="F147" s="9"/>
@@ -5140,11 +5368,13 @@
       <c r="X147" s="11"/>
       <c r="Y147" s="11"/>
     </row>
-    <row r="148" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B148" s="8">
         <v>44552</v>
       </c>
-      <c r="C148" s="9"/>
+      <c r="C148" s="9" t="s">
+        <v>134</v>
+      </c>
       <c r="D148" s="9"/>
       <c r="E148" s="9"/>
       <c r="F148" s="9"/>
@@ -5168,11 +5398,13 @@
       <c r="X148" s="11"/>
       <c r="Y148" s="11"/>
     </row>
-    <row r="149" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B149" s="8">
         <v>44553</v>
       </c>
-      <c r="C149" s="9"/>
+      <c r="C149" s="16" t="s">
+        <v>154</v>
+      </c>
       <c r="D149" s="9"/>
       <c r="E149" s="9"/>
       <c r="F149" s="9"/>
@@ -5196,11 +5428,13 @@
       <c r="X149" s="11"/>
       <c r="Y149" s="11"/>
     </row>
-    <row r="150" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B150" s="8">
         <v>44554</v>
       </c>
-      <c r="C150" s="9"/>
+      <c r="C150" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D150" s="9"/>
       <c r="E150" s="9"/>
       <c r="F150" s="9"/>
@@ -5224,7 +5458,7 @@
       <c r="X150" s="11"/>
       <c r="Y150" s="11"/>
     </row>
-    <row r="151" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B151" s="12">
         <v>44555</v>
       </c>
@@ -5252,7 +5486,7 @@
       <c r="X151" s="15"/>
       <c r="Y151" s="15"/>
     </row>
-    <row r="152" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B152" s="12">
         <v>44556</v>
       </c>
@@ -5280,11 +5514,16 @@
       <c r="X152" s="15"/>
       <c r="Y152" s="15"/>
     </row>
-    <row r="153" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>22</v>
+      </c>
       <c r="B153" s="8">
         <v>44557</v>
       </c>
-      <c r="C153" s="9"/>
+      <c r="C153" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D153" s="9"/>
       <c r="E153" s="9"/>
       <c r="F153" s="9"/>
@@ -5308,11 +5547,13 @@
       <c r="X153" s="11"/>
       <c r="Y153" s="11"/>
     </row>
-    <row r="154" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B154" s="8">
         <v>44558</v>
       </c>
-      <c r="C154" s="9"/>
+      <c r="C154" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D154" s="9"/>
       <c r="E154" s="9"/>
       <c r="F154" s="9"/>
@@ -5336,11 +5577,13 @@
       <c r="X154" s="11"/>
       <c r="Y154" s="11"/>
     </row>
-    <row r="155" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B155" s="8">
         <v>44559</v>
       </c>
-      <c r="C155" s="9"/>
+      <c r="C155" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D155" s="9"/>
       <c r="E155" s="9"/>
       <c r="F155" s="9"/>
@@ -5364,11 +5607,13 @@
       <c r="X155" s="11"/>
       <c r="Y155" s="11"/>
     </row>
-    <row r="156" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B156" s="8">
         <v>44560</v>
       </c>
-      <c r="C156" s="9"/>
+      <c r="C156" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D156" s="9"/>
       <c r="E156" s="9"/>
       <c r="F156" s="9"/>
@@ -5392,11 +5637,13 @@
       <c r="X156" s="11"/>
       <c r="Y156" s="11"/>
     </row>
-    <row r="157" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B157" s="8">
         <v>44561</v>
       </c>
-      <c r="C157" s="9"/>
+      <c r="C157" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="D157" s="9"/>
       <c r="E157" s="9"/>
       <c r="F157" s="9"/>
@@ -5420,7 +5667,7 @@
       <c r="X157" s="11"/>
       <c r="Y157" s="11"/>
     </row>
-    <row r="158" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B158" s="12">
         <v>44562</v>
       </c>
@@ -5448,7 +5695,7 @@
       <c r="X158" s="15"/>
       <c r="Y158" s="15"/>
     </row>
-    <row r="159" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B159" s="12">
         <v>44563</v>
       </c>
@@ -5476,11 +5723,16 @@
       <c r="X159" s="15"/>
       <c r="Y159" s="15"/>
     </row>
-    <row r="160" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A160">
+        <v>23</v>
+      </c>
       <c r="B160" s="8">
         <v>44564</v>
       </c>
-      <c r="C160" s="9"/>
+      <c r="C160" s="16" t="s">
+        <v>135</v>
+      </c>
       <c r="D160" s="9"/>
       <c r="E160" s="9"/>
       <c r="F160" s="9"/>
@@ -5504,11 +5756,13 @@
       <c r="X160" s="11"/>
       <c r="Y160" s="11"/>
     </row>
-    <row r="161" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B161" s="8">
         <v>44565</v>
       </c>
-      <c r="C161" s="9"/>
+      <c r="C161" s="16" t="s">
+        <v>137</v>
+      </c>
       <c r="D161" s="9"/>
       <c r="E161" s="9"/>
       <c r="F161" s="9"/>
@@ -5532,11 +5786,13 @@
       <c r="X161" s="11"/>
       <c r="Y161" s="11"/>
     </row>
-    <row r="162" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B162" s="8">
         <v>44566</v>
       </c>
-      <c r="C162" s="9"/>
+      <c r="C162" s="16" t="s">
+        <v>138</v>
+      </c>
       <c r="D162" s="9"/>
       <c r="E162" s="9"/>
       <c r="F162" s="9"/>
@@ -5560,11 +5816,13 @@
       <c r="X162" s="11"/>
       <c r="Y162" s="11"/>
     </row>
-    <row r="163" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B163" s="8">
         <v>44567</v>
       </c>
-      <c r="C163" s="9"/>
+      <c r="C163" s="16" t="s">
+        <v>139</v>
+      </c>
       <c r="D163" s="9"/>
       <c r="E163" s="9"/>
       <c r="F163" s="9"/>
@@ -5588,11 +5846,13 @@
       <c r="X163" s="11"/>
       <c r="Y163" s="11"/>
     </row>
-    <row r="164" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B164" s="8">
         <v>44568</v>
       </c>
-      <c r="C164" s="9"/>
+      <c r="C164" s="16" t="s">
+        <v>140</v>
+      </c>
       <c r="D164" s="9"/>
       <c r="E164" s="9"/>
       <c r="F164" s="9"/>
@@ -5616,7 +5876,7 @@
       <c r="X164" s="11"/>
       <c r="Y164" s="11"/>
     </row>
-    <row r="165" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B165" s="12">
         <v>44569</v>
       </c>
@@ -5644,7 +5904,7 @@
       <c r="X165" s="15"/>
       <c r="Y165" s="15"/>
     </row>
-    <row r="166" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B166" s="12">
         <v>44570</v>
       </c>
@@ -5672,11 +5932,16 @@
       <c r="X166" s="15"/>
       <c r="Y166" s="15"/>
     </row>
-    <row r="167" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>24</v>
+      </c>
       <c r="B167" s="8">
         <v>44571</v>
       </c>
-      <c r="C167" s="9"/>
+      <c r="C167" s="16" t="s">
+        <v>141</v>
+      </c>
       <c r="D167" s="9"/>
       <c r="E167" s="9"/>
       <c r="F167" s="9"/>
@@ -5700,11 +5965,13 @@
       <c r="X167" s="11"/>
       <c r="Y167" s="11"/>
     </row>
-    <row r="168" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B168" s="8">
         <v>44572</v>
       </c>
-      <c r="C168" s="9"/>
+      <c r="C168" s="16" t="s">
+        <v>142</v>
+      </c>
       <c r="D168" s="9"/>
       <c r="E168" s="9"/>
       <c r="F168" s="9"/>
@@ -5728,11 +5995,13 @@
       <c r="X168" s="11"/>
       <c r="Y168" s="11"/>
     </row>
-    <row r="169" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B169" s="8">
         <v>44573</v>
       </c>
-      <c r="C169" s="9"/>
+      <c r="C169" s="16" t="s">
+        <v>134</v>
+      </c>
       <c r="D169" s="9"/>
       <c r="E169" s="9"/>
       <c r="F169" s="9"/>
@@ -5756,11 +6025,13 @@
       <c r="X169" s="11"/>
       <c r="Y169" s="11"/>
     </row>
-    <row r="170" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B170" s="8">
         <v>44574</v>
       </c>
-      <c r="C170" s="9"/>
+      <c r="C170" s="16" t="s">
+        <v>144</v>
+      </c>
       <c r="D170" s="9"/>
       <c r="E170" s="9"/>
       <c r="F170" s="9"/>
@@ -5784,11 +6055,13 @@
       <c r="X170" s="11"/>
       <c r="Y170" s="11"/>
     </row>
-    <row r="171" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B171" s="8">
         <v>44575</v>
       </c>
-      <c r="C171" s="9"/>
+      <c r="C171" s="16" t="s">
+        <v>145</v>
+      </c>
       <c r="D171" s="9"/>
       <c r="E171" s="9"/>
       <c r="F171" s="9"/>
@@ -5812,7 +6085,7 @@
       <c r="X171" s="11"/>
       <c r="Y171" s="11"/>
     </row>
-    <row r="172" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B172" s="12">
         <v>44576</v>
       </c>
@@ -5840,7 +6113,7 @@
       <c r="X172" s="15"/>
       <c r="Y172" s="15"/>
     </row>
-    <row r="173" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B173" s="12">
         <v>44577</v>
       </c>
@@ -5868,11 +6141,16 @@
       <c r="X173" s="15"/>
       <c r="Y173" s="15"/>
     </row>
-    <row r="174" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>25</v>
+      </c>
       <c r="B174" s="8">
         <v>44578</v>
       </c>
-      <c r="C174" s="9"/>
+      <c r="C174" s="16" t="s">
+        <v>146</v>
+      </c>
       <c r="D174" s="9"/>
       <c r="E174" s="9"/>
       <c r="F174" s="9"/>
@@ -5896,11 +6174,13 @@
       <c r="X174" s="11"/>
       <c r="Y174" s="11"/>
     </row>
-    <row r="175" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B175" s="8">
         <v>44579</v>
       </c>
-      <c r="C175" s="9"/>
+      <c r="C175" s="16" t="s">
+        <v>147</v>
+      </c>
       <c r="D175" s="9"/>
       <c r="E175" s="9"/>
       <c r="F175" s="9"/>
@@ -5924,11 +6204,13 @@
       <c r="X175" s="11"/>
       <c r="Y175" s="11"/>
     </row>
-    <row r="176" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B176" s="8">
         <v>44580</v>
       </c>
-      <c r="C176" s="9"/>
+      <c r="C176" s="16" t="s">
+        <v>148</v>
+      </c>
       <c r="D176" s="9"/>
       <c r="E176" s="9"/>
       <c r="F176" s="9"/>
@@ -5952,11 +6234,13 @@
       <c r="X176" s="11"/>
       <c r="Y176" s="11"/>
     </row>
-    <row r="177" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B177" s="8">
         <v>44581</v>
       </c>
-      <c r="C177" s="9"/>
+      <c r="C177" s="16" t="s">
+        <v>149</v>
+      </c>
       <c r="D177" s="9"/>
       <c r="E177" s="9"/>
       <c r="F177" s="9"/>
@@ -5980,11 +6264,13 @@
       <c r="X177" s="11"/>
       <c r="Y177" s="11"/>
     </row>
-    <row r="178" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B178" s="8">
         <v>44582</v>
       </c>
-      <c r="C178" s="9"/>
+      <c r="C178" s="19" t="s">
+        <v>150</v>
+      </c>
       <c r="D178" s="9"/>
       <c r="E178" s="9"/>
       <c r="F178" s="9"/>
@@ -6008,7 +6294,7 @@
       <c r="X178" s="11"/>
       <c r="Y178" s="11"/>
     </row>
-    <row r="179" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B179" s="12">
         <v>44583</v>
       </c>
@@ -6036,7 +6322,7 @@
       <c r="X179" s="15"/>
       <c r="Y179" s="15"/>
     </row>
-    <row r="180" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B180" s="12">
         <v>44584</v>
       </c>
@@ -6064,11 +6350,16 @@
       <c r="X180" s="15"/>
       <c r="Y180" s="15"/>
     </row>
-    <row r="181" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>26</v>
+      </c>
       <c r="B181" s="8">
         <v>44585</v>
       </c>
-      <c r="C181" s="9"/>
+      <c r="C181" s="19" t="s">
+        <v>151</v>
+      </c>
       <c r="D181" s="9"/>
       <c r="E181" s="9"/>
       <c r="F181" s="9"/>
@@ -6092,11 +6383,13 @@
       <c r="X181" s="11"/>
       <c r="Y181" s="11"/>
     </row>
-    <row r="182" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B182" s="8">
         <v>44586</v>
       </c>
-      <c r="C182" s="9"/>
+      <c r="C182" s="19" t="s">
+        <v>151</v>
+      </c>
       <c r="D182" s="9"/>
       <c r="E182" s="9"/>
       <c r="F182" s="9"/>
@@ -6120,11 +6413,13 @@
       <c r="X182" s="11"/>
       <c r="Y182" s="11"/>
     </row>
-    <row r="183" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B183" s="8">
         <v>44587</v>
       </c>
-      <c r="C183" s="9"/>
+      <c r="C183" s="19" t="s">
+        <v>151</v>
+      </c>
       <c r="D183" s="9"/>
       <c r="E183" s="9"/>
       <c r="F183" s="9"/>
@@ -6148,11 +6443,13 @@
       <c r="X183" s="11"/>
       <c r="Y183" s="11"/>
     </row>
-    <row r="184" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B184" s="8">
         <v>44588</v>
       </c>
-      <c r="C184" s="9"/>
+      <c r="C184" s="16" t="s">
+        <v>152</v>
+      </c>
       <c r="D184" s="9"/>
       <c r="E184" s="9"/>
       <c r="F184" s="9"/>
@@ -6176,11 +6473,13 @@
       <c r="X184" s="11"/>
       <c r="Y184" s="11"/>
     </row>
-    <row r="185" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B185" s="8">
         <v>44589</v>
       </c>
-      <c r="C185" s="9"/>
+      <c r="C185" s="16" t="s">
+        <v>153</v>
+      </c>
       <c r="D185" s="9"/>
       <c r="E185" s="9"/>
       <c r="F185" s="9"/>
@@ -6204,7 +6503,7 @@
       <c r="X185" s="11"/>
       <c r="Y185" s="11"/>
     </row>
-    <row r="186" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B186" s="12">
         <v>44590</v>
       </c>
@@ -6232,7 +6531,7 @@
       <c r="X186" s="15"/>
       <c r="Y186" s="15"/>
     </row>
-    <row r="187" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B187" s="12">
         <v>44591</v>
       </c>
@@ -6260,11 +6559,16 @@
       <c r="X187" s="15"/>
       <c r="Y187" s="15"/>
     </row>
-    <row r="188" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A188">
+        <v>27</v>
+      </c>
       <c r="B188" s="8">
         <v>44592</v>
       </c>
-      <c r="C188" s="9"/>
+      <c r="C188" s="16" t="s">
+        <v>129</v>
+      </c>
       <c r="D188" s="9"/>
       <c r="E188" s="9"/>
       <c r="F188" s="9"/>
@@ -6288,11 +6592,13 @@
       <c r="X188" s="11"/>
       <c r="Y188" s="11"/>
     </row>
-    <row r="189" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B189" s="8">
         <v>44593</v>
       </c>
-      <c r="C189" s="9"/>
+      <c r="C189" s="16" t="s">
+        <v>128</v>
+      </c>
       <c r="D189" s="9"/>
       <c r="E189" s="9"/>
       <c r="F189" s="9"/>
@@ -6316,11 +6622,13 @@
       <c r="X189" s="11"/>
       <c r="Y189" s="11"/>
     </row>
-    <row r="190" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B190" s="8">
         <v>44594</v>
       </c>
-      <c r="C190" s="9"/>
+      <c r="C190" s="16" t="s">
+        <v>131</v>
+      </c>
       <c r="D190" s="9"/>
       <c r="E190" s="9"/>
       <c r="F190" s="9"/>
@@ -6344,11 +6652,13 @@
       <c r="X190" s="11"/>
       <c r="Y190" s="11"/>
     </row>
-    <row r="191" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B191" s="8">
         <v>44595</v>
       </c>
-      <c r="C191" s="9"/>
+      <c r="C191" s="16" t="s">
+        <v>127</v>
+      </c>
       <c r="D191" s="9"/>
       <c r="E191" s="9"/>
       <c r="F191" s="9"/>
@@ -6372,11 +6682,13 @@
       <c r="X191" s="11"/>
       <c r="Y191" s="11"/>
     </row>
-    <row r="192" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B192" s="8">
         <v>44596</v>
       </c>
-      <c r="C192" s="9"/>
+      <c r="C192" s="16" t="s">
+        <v>136</v>
+      </c>
       <c r="D192" s="9"/>
       <c r="E192" s="9"/>
       <c r="F192" s="9"/>
@@ -6400,7 +6712,7 @@
       <c r="X192" s="11"/>
       <c r="Y192" s="11"/>
     </row>
-    <row r="193" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B193" s="12">
         <v>44597</v>
       </c>
@@ -6428,7 +6740,7 @@
       <c r="X193" s="15"/>
       <c r="Y193" s="15"/>
     </row>
-    <row r="194" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B194" s="12">
         <v>44598</v>
       </c>
@@ -6456,11 +6768,16 @@
       <c r="X194" s="15"/>
       <c r="Y194" s="15"/>
     </row>
-    <row r="195" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A195">
+        <v>28</v>
+      </c>
       <c r="B195" s="8">
         <v>44599</v>
       </c>
-      <c r="C195" s="9"/>
+      <c r="C195" s="16" t="s">
+        <v>125</v>
+      </c>
       <c r="D195" s="9"/>
       <c r="E195" s="9"/>
       <c r="F195" s="9"/>
@@ -6484,11 +6801,13 @@
       <c r="X195" s="11"/>
       <c r="Y195" s="11"/>
     </row>
-    <row r="196" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B196" s="8">
         <v>44600</v>
       </c>
-      <c r="C196" s="9"/>
+      <c r="C196" s="16" t="s">
+        <v>126</v>
+      </c>
       <c r="D196" s="9"/>
       <c r="E196" s="9"/>
       <c r="F196" s="9"/>
@@ -6512,11 +6831,13 @@
       <c r="X196" s="11"/>
       <c r="Y196" s="11"/>
     </row>
-    <row r="197" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B197" s="8">
         <v>44601</v>
       </c>
-      <c r="C197" s="9"/>
+      <c r="C197" s="19" t="s">
+        <v>155</v>
+      </c>
       <c r="D197" s="9"/>
       <c r="E197" s="9"/>
       <c r="F197" s="9"/>
@@ -6540,11 +6861,13 @@
       <c r="X197" s="11"/>
       <c r="Y197" s="11"/>
     </row>
-    <row r="198" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B198" s="8">
         <v>44602</v>
       </c>
-      <c r="C198" s="9"/>
+      <c r="C198" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="D198" s="9"/>
       <c r="E198" s="9"/>
       <c r="F198" s="9"/>
@@ -6568,11 +6891,13 @@
       <c r="X198" s="11"/>
       <c r="Y198" s="11"/>
     </row>
-    <row r="199" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B199" s="8">
         <v>44603</v>
       </c>
-      <c r="C199" s="9"/>
+      <c r="C199" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="D199" s="9"/>
       <c r="E199" s="9"/>
       <c r="F199" s="9"/>
@@ -6596,7 +6921,7 @@
       <c r="X199" s="11"/>
       <c r="Y199" s="11"/>
     </row>
-    <row r="200" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B200" s="12">
         <v>44604</v>
       </c>
@@ -6624,7 +6949,7 @@
       <c r="X200" s="15"/>
       <c r="Y200" s="15"/>
     </row>
-    <row r="201" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B201" s="12">
         <v>44605</v>
       </c>
@@ -6652,11 +6977,16 @@
       <c r="X201" s="15"/>
       <c r="Y201" s="15"/>
     </row>
-    <row r="202" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>29</v>
+      </c>
       <c r="B202" s="8">
         <v>44606</v>
       </c>
-      <c r="C202" s="9"/>
+      <c r="C202" s="16" t="s">
+        <v>121</v>
+      </c>
       <c r="D202" s="9"/>
       <c r="E202" s="9"/>
       <c r="F202" s="9"/>
@@ -6680,11 +7010,13 @@
       <c r="X202" s="11"/>
       <c r="Y202" s="11"/>
     </row>
-    <row r="203" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B203" s="8">
         <v>44607</v>
       </c>
-      <c r="C203" s="9"/>
+      <c r="C203" s="16" t="s">
+        <v>122</v>
+      </c>
       <c r="D203" s="9"/>
       <c r="E203" s="9"/>
       <c r="F203" s="9"/>
@@ -6708,11 +7040,13 @@
       <c r="X203" s="11"/>
       <c r="Y203" s="11"/>
     </row>
-    <row r="204" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B204" s="8">
         <v>44608</v>
       </c>
-      <c r="C204" s="9"/>
+      <c r="C204" s="16" t="s">
+        <v>123</v>
+      </c>
       <c r="D204" s="9"/>
       <c r="E204" s="9"/>
       <c r="F204" s="9"/>
@@ -6736,11 +7070,13 @@
       <c r="X204" s="11"/>
       <c r="Y204" s="11"/>
     </row>
-    <row r="205" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B205" s="8">
         <v>44609</v>
       </c>
-      <c r="C205" s="9"/>
+      <c r="C205" s="16" t="s">
+        <v>124</v>
+      </c>
       <c r="D205" s="9"/>
       <c r="E205" s="9"/>
       <c r="F205" s="9"/>
@@ -6764,11 +7100,13 @@
       <c r="X205" s="11"/>
       <c r="Y205" s="11"/>
     </row>
-    <row r="206" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B206" s="8">
         <v>44610</v>
       </c>
-      <c r="C206" s="9"/>
+      <c r="C206" s="16" t="s">
+        <v>130</v>
+      </c>
       <c r="D206" s="9"/>
       <c r="E206" s="9"/>
       <c r="F206" s="9"/>
@@ -6792,7 +7130,7 @@
       <c r="X206" s="11"/>
       <c r="Y206" s="11"/>
     </row>
-    <row r="207" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B207" s="12">
         <v>44611</v>
       </c>
@@ -6820,7 +7158,7 @@
       <c r="X207" s="15"/>
       <c r="Y207" s="15"/>
     </row>
-    <row r="208" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B208" s="12">
         <v>44612</v>
       </c>
@@ -6848,11 +7186,16 @@
       <c r="X208" s="15"/>
       <c r="Y208" s="15"/>
     </row>
-    <row r="209" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>30</v>
+      </c>
       <c r="B209" s="8">
         <v>44613</v>
       </c>
-      <c r="C209" s="9"/>
+      <c r="C209" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="D209" s="9"/>
       <c r="E209" s="9"/>
       <c r="F209" s="9"/>
@@ -6876,11 +7219,13 @@
       <c r="X209" s="11"/>
       <c r="Y209" s="11"/>
     </row>
-    <row r="210" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B210" s="8">
         <v>44614</v>
       </c>
-      <c r="C210" s="9"/>
+      <c r="C210" s="16" t="s">
+        <v>120</v>
+      </c>
       <c r="D210" s="9"/>
       <c r="E210" s="9"/>
       <c r="F210" s="9"/>
@@ -6904,11 +7249,13 @@
       <c r="X210" s="11"/>
       <c r="Y210" s="11"/>
     </row>
-    <row r="211" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B211" s="8">
         <v>44615</v>
       </c>
-      <c r="C211" s="9"/>
+      <c r="C211" s="16" t="s">
+        <v>118</v>
+      </c>
       <c r="D211" s="9"/>
       <c r="E211" s="9"/>
       <c r="F211" s="9"/>
@@ -6932,11 +7279,13 @@
       <c r="X211" s="11"/>
       <c r="Y211" s="11"/>
     </row>
-    <row r="212" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B212" s="8">
         <v>44616</v>
       </c>
-      <c r="C212" s="9"/>
+      <c r="C212" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="D212" s="9"/>
       <c r="E212" s="9"/>
       <c r="F212" s="9"/>
@@ -6960,11 +7309,13 @@
       <c r="X212" s="11"/>
       <c r="Y212" s="11"/>
     </row>
-    <row r="213" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B213" s="8">
         <v>44617</v>
       </c>
-      <c r="C213" s="9"/>
+      <c r="C213" s="16" t="s">
+        <v>116</v>
+      </c>
       <c r="D213" s="9"/>
       <c r="E213" s="9"/>
       <c r="F213" s="9"/>
@@ -6988,7 +7339,7 @@
       <c r="X213" s="11"/>
       <c r="Y213" s="11"/>
     </row>
-    <row r="214" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B214" s="12">
         <v>44618</v>
       </c>
@@ -7016,7 +7367,7 @@
       <c r="X214" s="15"/>
       <c r="Y214" s="15"/>
     </row>
-    <row r="215" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B215" s="12">
         <v>44619</v>
       </c>
@@ -7044,11 +7395,16 @@
       <c r="X215" s="15"/>
       <c r="Y215" s="15"/>
     </row>
-    <row r="216" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A216">
+        <v>31</v>
+      </c>
       <c r="B216" s="8">
         <v>44620</v>
       </c>
-      <c r="C216" s="9"/>
+      <c r="C216" s="16" t="s">
+        <v>115</v>
+      </c>
       <c r="D216" s="9"/>
       <c r="E216" s="9"/>
       <c r="F216" s="9"/>
@@ -7072,11 +7428,13 @@
       <c r="X216" s="11"/>
       <c r="Y216" s="11"/>
     </row>
-    <row r="217" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B217" s="8">
         <v>44621</v>
       </c>
-      <c r="C217" s="9"/>
+      <c r="C217" s="16" t="s">
+        <v>143</v>
+      </c>
       <c r="D217" s="9"/>
       <c r="E217" s="9"/>
       <c r="F217" s="9"/>
@@ -7100,7 +7458,7 @@
       <c r="X217" s="11"/>
       <c r="Y217" s="11"/>
     </row>
-    <row r="218" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B218" s="8">
         <v>44622</v>
       </c>
@@ -7128,7 +7486,7 @@
       <c r="X218" s="11"/>
       <c r="Y218" s="11"/>
     </row>
-    <row r="219" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B219" s="8">
         <v>44623</v>
       </c>
@@ -7156,7 +7514,7 @@
       <c r="X219" s="11"/>
       <c r="Y219" s="11"/>
     </row>
-    <row r="220" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B220" s="8">
         <v>44624</v>
       </c>
@@ -7184,7 +7542,7 @@
       <c r="X220" s="11"/>
       <c r="Y220" s="11"/>
     </row>
-    <row r="221" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B221" s="12">
         <v>44625</v>
       </c>
@@ -7212,7 +7570,7 @@
       <c r="X221" s="15"/>
       <c r="Y221" s="15"/>
     </row>
-    <row r="222" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B222" s="12">
         <v>44626</v>
       </c>
@@ -7240,7 +7598,10 @@
       <c r="X222" s="15"/>
       <c r="Y222" s="15"/>
     </row>
-    <row r="223" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A223">
+        <v>32</v>
+      </c>
       <c r="B223" s="8">
         <v>44627</v>
       </c>
@@ -7268,7 +7629,7 @@
       <c r="X223" s="11"/>
       <c r="Y223" s="11"/>
     </row>
-    <row r="224" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B224" s="8">
         <v>44628</v>
       </c>
@@ -7296,7 +7657,7 @@
       <c r="X224" s="11"/>
       <c r="Y224" s="11"/>
     </row>
-    <row r="225" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B225" s="8">
         <v>44629</v>
       </c>
@@ -7324,7 +7685,7 @@
       <c r="X225" s="11"/>
       <c r="Y225" s="11"/>
     </row>
-    <row r="226" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B226" s="8">
         <v>44630</v>
       </c>
@@ -7352,7 +7713,7 @@
       <c r="X226" s="11"/>
       <c r="Y226" s="11"/>
     </row>
-    <row r="227" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B227" s="8">
         <v>44631</v>
       </c>
@@ -7380,7 +7741,7 @@
       <c r="X227" s="11"/>
       <c r="Y227" s="11"/>
     </row>
-    <row r="228" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B228" s="12">
         <v>44632</v>
       </c>
@@ -7408,7 +7769,7 @@
       <c r="X228" s="15"/>
       <c r="Y228" s="15"/>
     </row>
-    <row r="229" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B229" s="12">
         <v>44633</v>
       </c>
@@ -7436,7 +7797,10 @@
       <c r="X229" s="15"/>
       <c r="Y229" s="15"/>
     </row>
-    <row r="230" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A230">
+        <v>33</v>
+      </c>
       <c r="B230" s="8">
         <v>44634</v>
       </c>
@@ -7464,7 +7828,7 @@
       <c r="X230" s="11"/>
       <c r="Y230" s="11"/>
     </row>
-    <row r="231" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B231" s="8">
         <v>44635</v>
       </c>
@@ -7492,7 +7856,7 @@
       <c r="X231" s="11"/>
       <c r="Y231" s="11"/>
     </row>
-    <row r="232" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B232" s="8">
         <v>44636</v>
       </c>
@@ -7520,7 +7884,7 @@
       <c r="X232" s="11"/>
       <c r="Y232" s="11"/>
     </row>
-    <row r="233" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B233" s="8">
         <v>44637</v>
       </c>
@@ -7548,7 +7912,7 @@
       <c r="X233" s="11"/>
       <c r="Y233" s="11"/>
     </row>
-    <row r="234" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B234" s="8">
         <v>44638</v>
       </c>
@@ -7576,7 +7940,7 @@
       <c r="X234" s="11"/>
       <c r="Y234" s="11"/>
     </row>
-    <row r="235" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B235" s="12">
         <v>44639</v>
       </c>
@@ -7604,7 +7968,7 @@
       <c r="X235" s="15"/>
       <c r="Y235" s="15"/>
     </row>
-    <row r="236" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B236" s="12">
         <v>44640</v>
       </c>
@@ -7632,7 +7996,10 @@
       <c r="X236" s="15"/>
       <c r="Y236" s="15"/>
     </row>
-    <row r="237" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A237">
+        <v>34</v>
+      </c>
       <c r="B237" s="8">
         <v>44641</v>
       </c>
@@ -7660,7 +8027,7 @@
       <c r="X237" s="11"/>
       <c r="Y237" s="11"/>
     </row>
-    <row r="238" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B238" s="8">
         <v>44642</v>
       </c>
@@ -7688,7 +8055,7 @@
       <c r="X238" s="11"/>
       <c r="Y238" s="11"/>
     </row>
-    <row r="239" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B239" s="8">
         <v>44643</v>
       </c>
@@ -7716,7 +8083,7 @@
       <c r="X239" s="11"/>
       <c r="Y239" s="11"/>
     </row>
-    <row r="240" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B240" s="8">
         <v>44644</v>
       </c>
@@ -7744,7 +8111,7 @@
       <c r="X240" s="11"/>
       <c r="Y240" s="11"/>
     </row>
-    <row r="241" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B241" s="8">
         <v>44645</v>
       </c>
@@ -7772,7 +8139,7 @@
       <c r="X241" s="11"/>
       <c r="Y241" s="11"/>
     </row>
-    <row r="242" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B242" s="12">
         <v>44646</v>
       </c>
@@ -7800,7 +8167,7 @@
       <c r="X242" s="15"/>
       <c r="Y242" s="15"/>
     </row>
-    <row r="243" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B243" s="12">
         <v>44647</v>
       </c>
@@ -7828,7 +8195,10 @@
       <c r="X243" s="15"/>
       <c r="Y243" s="15"/>
     </row>
-    <row r="244" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A244">
+        <v>35</v>
+      </c>
       <c r="B244" s="8">
         <v>44648</v>
       </c>
@@ -7856,7 +8226,7 @@
       <c r="X244" s="11"/>
       <c r="Y244" s="11"/>
     </row>
-    <row r="245" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B245" s="8">
         <v>44649</v>
       </c>
@@ -7884,7 +8254,7 @@
       <c r="X245" s="11"/>
       <c r="Y245" s="11"/>
     </row>
-    <row r="246" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B246" s="8">
         <v>44650</v>
       </c>
@@ -7912,7 +8282,7 @@
       <c r="X246" s="11"/>
       <c r="Y246" s="11"/>
     </row>
-    <row r="247" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B247" s="8">
         <v>44651</v>
       </c>
@@ -7940,7 +8310,7 @@
       <c r="X247" s="11"/>
       <c r="Y247" s="11"/>
     </row>
-    <row r="248" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B248" s="8">
         <v>44652</v>
       </c>
@@ -7968,7 +8338,7 @@
       <c r="X248" s="11"/>
       <c r="Y248" s="11"/>
     </row>
-    <row r="249" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B249" s="12">
         <v>44653</v>
       </c>
@@ -7996,7 +8366,7 @@
       <c r="X249" s="15"/>
       <c r="Y249" s="15"/>
     </row>
-    <row r="250" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B250" s="12">
         <v>44654</v>
       </c>
@@ -8024,7 +8394,10 @@
       <c r="X250" s="15"/>
       <c r="Y250" s="15"/>
     </row>
-    <row r="251" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A251">
+        <v>36</v>
+      </c>
       <c r="B251" s="8">
         <v>44655</v>
       </c>
@@ -8052,7 +8425,7 @@
       <c r="X251" s="11"/>
       <c r="Y251" s="11"/>
     </row>
-    <row r="252" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B252" s="8">
         <v>44656</v>
       </c>
@@ -8080,7 +8453,7 @@
       <c r="X252" s="11"/>
       <c r="Y252" s="11"/>
     </row>
-    <row r="253" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B253" s="8">
         <v>44657</v>
       </c>
@@ -8108,7 +8481,7 @@
       <c r="X253" s="11"/>
       <c r="Y253" s="11"/>
     </row>
-    <row r="254" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B254" s="8">
         <v>44658</v>
       </c>
@@ -8136,7 +8509,7 @@
       <c r="X254" s="11"/>
       <c r="Y254" s="11"/>
     </row>
-    <row r="255" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B255" s="8">
         <v>44659</v>
       </c>
@@ -8164,7 +8537,7 @@
       <c r="X255" s="11"/>
       <c r="Y255" s="11"/>
     </row>
-    <row r="256" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B256" s="12">
         <v>44660</v>
       </c>
@@ -8192,7 +8565,7 @@
       <c r="X256" s="15"/>
       <c r="Y256" s="15"/>
     </row>
-    <row r="257" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B257" s="12">
         <v>44661</v>
       </c>
@@ -8220,7 +8593,10 @@
       <c r="X257" s="15"/>
       <c r="Y257" s="15"/>
     </row>
-    <row r="258" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A258">
+        <v>37</v>
+      </c>
       <c r="B258" s="8">
         <v>44662</v>
       </c>
@@ -8248,7 +8624,7 @@
       <c r="X258" s="11"/>
       <c r="Y258" s="11"/>
     </row>
-    <row r="259" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B259" s="8">
         <v>44663</v>
       </c>
@@ -8276,7 +8652,7 @@
       <c r="X259" s="11"/>
       <c r="Y259" s="11"/>
     </row>
-    <row r="260" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B260" s="8">
         <v>44664</v>
       </c>
@@ -8304,7 +8680,7 @@
       <c r="X260" s="11"/>
       <c r="Y260" s="11"/>
     </row>
-    <row r="261" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B261" s="8">
         <v>44665</v>
       </c>
@@ -8332,7 +8708,7 @@
       <c r="X261" s="11"/>
       <c r="Y261" s="11"/>
     </row>
-    <row r="262" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B262" s="8">
         <v>44666</v>
       </c>
@@ -8360,7 +8736,7 @@
       <c r="X262" s="11"/>
       <c r="Y262" s="11"/>
     </row>
-    <row r="263" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B263" s="12">
         <v>44667</v>
       </c>
@@ -8388,7 +8764,7 @@
       <c r="X263" s="15"/>
       <c r="Y263" s="15"/>
     </row>
-    <row r="264" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B264" s="12">
         <v>44668</v>
       </c>
@@ -8416,7 +8792,10 @@
       <c r="X264" s="15"/>
       <c r="Y264" s="15"/>
     </row>
-    <row r="265" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A265">
+        <v>38</v>
+      </c>
       <c r="B265" s="8">
         <v>44669</v>
       </c>
@@ -8444,7 +8823,7 @@
       <c r="X265" s="11"/>
       <c r="Y265" s="11"/>
     </row>
-    <row r="266" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B266" s="8">
         <v>44670</v>
       </c>
@@ -8472,7 +8851,7 @@
       <c r="X266" s="11"/>
       <c r="Y266" s="11"/>
     </row>
-    <row r="267" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B267" s="8">
         <v>44671</v>
       </c>
@@ -8500,7 +8879,7 @@
       <c r="X267" s="11"/>
       <c r="Y267" s="11"/>
     </row>
-    <row r="268" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B268" s="8">
         <v>44672</v>
       </c>
@@ -8528,7 +8907,7 @@
       <c r="X268" s="11"/>
       <c r="Y268" s="11"/>
     </row>
-    <row r="269" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B269" s="8">
         <v>44673</v>
       </c>
@@ -8556,7 +8935,7 @@
       <c r="X269" s="11"/>
       <c r="Y269" s="11"/>
     </row>
-    <row r="270" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B270" s="12">
         <v>44674</v>
       </c>
@@ -8584,7 +8963,7 @@
       <c r="X270" s="15"/>
       <c r="Y270" s="15"/>
     </row>
-    <row r="271" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B271" s="12">
         <v>44675</v>
       </c>
@@ -8612,7 +8991,10 @@
       <c r="X271" s="15"/>
       <c r="Y271" s="15"/>
     </row>
-    <row r="272" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A272">
+        <v>39</v>
+      </c>
       <c r="B272" s="8">
         <v>44676</v>
       </c>
@@ -8640,7 +9022,7 @@
       <c r="X272" s="11"/>
       <c r="Y272" s="11"/>
     </row>
-    <row r="273" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B273" s="8">
         <v>44677</v>
       </c>
@@ -8668,7 +9050,7 @@
       <c r="X273" s="11"/>
       <c r="Y273" s="11"/>
     </row>
-    <row r="274" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B274" s="8">
         <v>44678</v>
       </c>
@@ -8696,7 +9078,7 @@
       <c r="X274" s="11"/>
       <c r="Y274" s="11"/>
     </row>
-    <row r="275" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B275" s="8">
         <v>44679</v>
       </c>
@@ -8724,7 +9106,7 @@
       <c r="X275" s="11"/>
       <c r="Y275" s="11"/>
     </row>
-    <row r="276" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B276" s="8">
         <v>44680</v>
       </c>
@@ -8752,7 +9134,7 @@
       <c r="X276" s="11"/>
       <c r="Y276" s="11"/>
     </row>
-    <row r="277" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B277" s="12">
         <v>44681</v>
       </c>
@@ -8780,7 +9162,7 @@
       <c r="X277" s="15"/>
       <c r="Y277" s="15"/>
     </row>
-    <row r="278" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B278" s="12">
         <v>44682</v>
       </c>
@@ -8808,7 +9190,10 @@
       <c r="X278" s="15"/>
       <c r="Y278" s="15"/>
     </row>
-    <row r="279" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>40</v>
+      </c>
       <c r="B279" s="8">
         <v>44683</v>
       </c>
@@ -8836,7 +9221,7 @@
       <c r="X279" s="11"/>
       <c r="Y279" s="11"/>
     </row>
-    <row r="280" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B280" s="8">
         <v>44684</v>
       </c>
@@ -8864,7 +9249,7 @@
       <c r="X280" s="11"/>
       <c r="Y280" s="11"/>
     </row>
-    <row r="281" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B281" s="8">
         <v>44685</v>
       </c>
@@ -8892,7 +9277,7 @@
       <c r="X281" s="11"/>
       <c r="Y281" s="11"/>
     </row>
-    <row r="282" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B282" s="8">
         <v>44686</v>
       </c>
@@ -8920,7 +9305,7 @@
       <c r="X282" s="11"/>
       <c r="Y282" s="11"/>
     </row>
-    <row r="283" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B283" s="8">
         <v>44687</v>
       </c>
@@ -8948,7 +9333,7 @@
       <c r="X283" s="11"/>
       <c r="Y283" s="11"/>
     </row>
-    <row r="284" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B284" s="12">
         <v>44688</v>
       </c>
@@ -8976,7 +9361,7 @@
       <c r="X284" s="15"/>
       <c r="Y284" s="15"/>
     </row>
-    <row r="285" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B285" s="12">
         <v>44689</v>
       </c>
@@ -9004,7 +9389,10 @@
       <c r="X285" s="15"/>
       <c r="Y285" s="15"/>
     </row>
-    <row r="286" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>41</v>
+      </c>
       <c r="B286" s="8">
         <v>44690</v>
       </c>
@@ -9032,7 +9420,7 @@
       <c r="X286" s="11"/>
       <c r="Y286" s="11"/>
     </row>
-    <row r="287" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B287" s="8">
         <v>44691</v>
       </c>
@@ -9060,7 +9448,7 @@
       <c r="X287" s="11"/>
       <c r="Y287" s="11"/>
     </row>
-    <row r="288" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B288" s="8">
         <v>44692</v>
       </c>
@@ -9088,7 +9476,7 @@
       <c r="X288" s="11"/>
       <c r="Y288" s="11"/>
     </row>
-    <row r="289" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B289" s="8">
         <v>44693</v>
       </c>
@@ -9116,7 +9504,7 @@
       <c r="X289" s="11"/>
       <c r="Y289" s="11"/>
     </row>
-    <row r="290" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B290" s="8">
         <v>44694</v>
       </c>
@@ -9144,7 +9532,7 @@
       <c r="X290" s="11"/>
       <c r="Y290" s="11"/>
     </row>
-    <row r="291" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B291" s="12">
         <v>44695</v>
       </c>
@@ -9172,7 +9560,7 @@
       <c r="X291" s="15"/>
       <c r="Y291" s="15"/>
     </row>
-    <row r="292" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B292" s="12">
         <v>44696</v>
       </c>
@@ -9200,7 +9588,10 @@
       <c r="X292" s="15"/>
       <c r="Y292" s="15"/>
     </row>
-    <row r="293" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>42</v>
+      </c>
       <c r="B293" s="8">
         <v>44697</v>
       </c>
@@ -9228,7 +9619,7 @@
       <c r="X293" s="11"/>
       <c r="Y293" s="11"/>
     </row>
-    <row r="294" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B294" s="8">
         <v>44698</v>
       </c>
@@ -9256,7 +9647,7 @@
       <c r="X294" s="11"/>
       <c r="Y294" s="11"/>
     </row>
-    <row r="295" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B295" s="8">
         <v>44699</v>
       </c>
@@ -9284,7 +9675,7 @@
       <c r="X295" s="11"/>
       <c r="Y295" s="11"/>
     </row>
-    <row r="296" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B296" s="8">
         <v>44700</v>
       </c>
@@ -9312,7 +9703,7 @@
       <c r="X296" s="11"/>
       <c r="Y296" s="11"/>
     </row>
-    <row r="297" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B297" s="8">
         <v>44701</v>
       </c>
@@ -9340,7 +9731,7 @@
       <c r="X297" s="11"/>
       <c r="Y297" s="11"/>
     </row>
-    <row r="298" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B298" s="12">
         <v>44702</v>
       </c>
@@ -9368,7 +9759,7 @@
       <c r="X298" s="15"/>
       <c r="Y298" s="15"/>
     </row>
-    <row r="299" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B299" s="12">
         <v>44703</v>
       </c>
@@ -9396,7 +9787,10 @@
       <c r="X299" s="15"/>
       <c r="Y299" s="15"/>
     </row>
-    <row r="300" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>43</v>
+      </c>
       <c r="B300" s="8">
         <v>44704</v>
       </c>
@@ -9424,7 +9818,7 @@
       <c r="X300" s="11"/>
       <c r="Y300" s="11"/>
     </row>
-    <row r="301" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B301" s="8">
         <v>44705</v>
       </c>
@@ -9452,7 +9846,7 @@
       <c r="X301" s="11"/>
       <c r="Y301" s="11"/>
     </row>
-    <row r="302" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B302" s="8">
         <v>44706</v>
       </c>
@@ -9480,7 +9874,7 @@
       <c r="X302" s="11"/>
       <c r="Y302" s="11"/>
     </row>
-    <row r="303" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B303" s="8">
         <v>44707</v>
       </c>
@@ -9508,7 +9902,7 @@
       <c r="X303" s="11"/>
       <c r="Y303" s="11"/>
     </row>
-    <row r="304" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B304" s="8">
         <v>44708</v>
       </c>
@@ -9536,7 +9930,7 @@
       <c r="X304" s="11"/>
       <c r="Y304" s="11"/>
     </row>
-    <row r="305" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B305" s="12">
         <v>44709</v>
       </c>
@@ -9564,7 +9958,7 @@
       <c r="X305" s="15"/>
       <c r="Y305" s="15"/>
     </row>
-    <row r="306" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B306" s="12">
         <v>44710</v>
       </c>
@@ -9592,7 +9986,10 @@
       <c r="X306" s="15"/>
       <c r="Y306" s="15"/>
     </row>
-    <row r="307" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>44</v>
+      </c>
       <c r="B307" s="8">
         <v>44711</v>
       </c>
@@ -9620,7 +10017,7 @@
       <c r="X307" s="11"/>
       <c r="Y307" s="11"/>
     </row>
-    <row r="308" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B308" s="8">
         <v>44712</v>
       </c>
@@ -9648,7 +10045,7 @@
       <c r="X308" s="11"/>
       <c r="Y308" s="11"/>
     </row>
-    <row r="309" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B309" s="8">
         <v>44713</v>
       </c>
@@ -9676,7 +10073,7 @@
       <c r="X309" s="11"/>
       <c r="Y309" s="11"/>
     </row>
-    <row r="310" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B310" s="8">
         <v>44714</v>
       </c>
@@ -9704,7 +10101,7 @@
       <c r="X310" s="11"/>
       <c r="Y310" s="11"/>
     </row>
-    <row r="311" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B311" s="8">
         <v>44715</v>
       </c>
@@ -9732,7 +10129,7 @@
       <c r="X311" s="11"/>
       <c r="Y311" s="11"/>
     </row>
-    <row r="312" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B312" s="12">
         <v>44716</v>
       </c>
@@ -9760,7 +10157,7 @@
       <c r="X312" s="15"/>
       <c r="Y312" s="15"/>
     </row>
-    <row r="313" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B313" s="12">
         <v>44717</v>
       </c>
@@ -9788,7 +10185,10 @@
       <c r="X313" s="15"/>
       <c r="Y313" s="15"/>
     </row>
-    <row r="314" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>45</v>
+      </c>
       <c r="B314" s="8">
         <v>44718</v>
       </c>
@@ -9816,7 +10216,7 @@
       <c r="X314" s="11"/>
       <c r="Y314" s="11"/>
     </row>
-    <row r="315" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B315" s="8">
         <v>44719</v>
       </c>
@@ -9844,7 +10244,7 @@
       <c r="X315" s="11"/>
       <c r="Y315" s="11"/>
     </row>
-    <row r="316" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B316" s="8">
         <v>44720</v>
       </c>
@@ -9872,7 +10272,7 @@
       <c r="X316" s="11"/>
       <c r="Y316" s="11"/>
     </row>
-    <row r="317" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B317" s="8">
         <v>44721</v>
       </c>
@@ -9900,7 +10300,7 @@
       <c r="X317" s="11"/>
       <c r="Y317" s="11"/>
     </row>
-    <row r="318" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B318" s="8">
         <v>44722</v>
       </c>
@@ -9928,7 +10328,7 @@
       <c r="X318" s="11"/>
       <c r="Y318" s="11"/>
     </row>
-    <row r="319" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B319" s="12">
         <v>44723</v>
       </c>
@@ -9956,7 +10356,7 @@
       <c r="X319" s="15"/>
       <c r="Y319" s="15"/>
     </row>
-    <row r="320" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B320" s="12">
         <v>44724</v>
       </c>
@@ -9984,7 +10384,10 @@
       <c r="X320" s="15"/>
       <c r="Y320" s="15"/>
     </row>
-    <row r="321" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>46</v>
+      </c>
       <c r="B321" s="8">
         <v>44725</v>
       </c>
@@ -10012,7 +10415,7 @@
       <c r="X321" s="11"/>
       <c r="Y321" s="11"/>
     </row>
-    <row r="322" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B322" s="8">
         <v>44726</v>
       </c>
@@ -10040,7 +10443,7 @@
       <c r="X322" s="11"/>
       <c r="Y322" s="11"/>
     </row>
-    <row r="323" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B323" s="8">
         <v>44727</v>
       </c>
@@ -10068,7 +10471,7 @@
       <c r="X323" s="11"/>
       <c r="Y323" s="11"/>
     </row>
-    <row r="324" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B324" s="8">
         <v>44728</v>
       </c>
@@ -10096,7 +10499,7 @@
       <c r="X324" s="11"/>
       <c r="Y324" s="11"/>
     </row>
-    <row r="325" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B325" s="8">
         <v>44729</v>
       </c>
@@ -10124,7 +10527,7 @@
       <c r="X325" s="11"/>
       <c r="Y325" s="11"/>
     </row>
-    <row r="326" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B326" s="12">
         <v>44730</v>
       </c>
@@ -10152,7 +10555,7 @@
       <c r="X326" s="15"/>
       <c r="Y326" s="15"/>
     </row>
-    <row r="327" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B327" s="12">
         <v>44731</v>
       </c>
@@ -10180,7 +10583,10 @@
       <c r="X327" s="15"/>
       <c r="Y327" s="15"/>
     </row>
-    <row r="328" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>47</v>
+      </c>
       <c r="B328" s="8">
         <v>44732</v>
       </c>
@@ -10208,7 +10614,7 @@
       <c r="X328" s="11"/>
       <c r="Y328" s="11"/>
     </row>
-    <row r="329" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B329" s="8">
         <v>44733</v>
       </c>
@@ -10236,7 +10642,7 @@
       <c r="X329" s="11"/>
       <c r="Y329" s="11"/>
     </row>
-    <row r="330" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B330" s="8">
         <v>44734</v>
       </c>
@@ -10264,7 +10670,7 @@
       <c r="X330" s="11"/>
       <c r="Y330" s="11"/>
     </row>
-    <row r="331" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B331" s="8">
         <v>44735</v>
       </c>
@@ -10292,7 +10698,7 @@
       <c r="X331" s="11"/>
       <c r="Y331" s="11"/>
     </row>
-    <row r="332" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B332" s="8">
         <v>44736</v>
       </c>
@@ -10320,7 +10726,7 @@
       <c r="X332" s="11"/>
       <c r="Y332" s="11"/>
     </row>
-    <row r="333" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B333" s="12">
         <v>44737</v>
       </c>
@@ -10348,7 +10754,7 @@
       <c r="X333" s="15"/>
       <c r="Y333" s="15"/>
     </row>
-    <row r="334" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B334" s="12">
         <v>44738</v>
       </c>
@@ -10376,7 +10782,10 @@
       <c r="X334" s="15"/>
       <c r="Y334" s="15"/>
     </row>
-    <row r="335" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>48</v>
+      </c>
       <c r="B335" s="8">
         <v>44739</v>
       </c>
@@ -10404,7 +10813,7 @@
       <c r="X335" s="11"/>
       <c r="Y335" s="11"/>
     </row>
-    <row r="336" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B336" s="8">
         <v>44740</v>
       </c>
@@ -10432,7 +10841,7 @@
       <c r="X336" s="11"/>
       <c r="Y336" s="11"/>
     </row>
-    <row r="337" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B337" s="8">
         <v>44741</v>
       </c>
@@ -10460,7 +10869,7 @@
       <c r="X337" s="11"/>
       <c r="Y337" s="11"/>
     </row>
-    <row r="338" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B338" s="8">
         <v>44742</v>
       </c>
@@ -10488,7 +10897,7 @@
       <c r="X338" s="11"/>
       <c r="Y338" s="11"/>
     </row>
-    <row r="339" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B339" s="8">
         <v>44743</v>
       </c>
@@ -10516,7 +10925,7 @@
       <c r="X339" s="11"/>
       <c r="Y339" s="11"/>
     </row>
-    <row r="340" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B340" s="12">
         <v>44744</v>
       </c>
@@ -10544,7 +10953,7 @@
       <c r="X340" s="15"/>
       <c r="Y340" s="15"/>
     </row>
-    <row r="341" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B341" s="12">
         <v>44745</v>
       </c>
@@ -10572,7 +10981,10 @@
       <c r="X341" s="15"/>
       <c r="Y341" s="15"/>
     </row>
-    <row r="342" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>49</v>
+      </c>
       <c r="B342" s="8">
         <v>44746</v>
       </c>
@@ -10600,7 +11012,7 @@
       <c r="X342" s="11"/>
       <c r="Y342" s="11"/>
     </row>
-    <row r="343" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B343" s="8">
         <v>44747</v>
       </c>
@@ -10628,7 +11040,7 @@
       <c r="X343" s="11"/>
       <c r="Y343" s="11"/>
     </row>
-    <row r="344" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B344" s="8">
         <v>44748</v>
       </c>
@@ -10656,7 +11068,7 @@
       <c r="X344" s="11"/>
       <c r="Y344" s="11"/>
     </row>
-    <row r="345" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B345" s="8">
         <v>44749</v>
       </c>
@@ -10684,7 +11096,7 @@
       <c r="X345" s="11"/>
       <c r="Y345" s="11"/>
     </row>
-    <row r="346" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B346" s="8">
         <v>44750</v>
       </c>
@@ -10712,7 +11124,7 @@
       <c r="X346" s="11"/>
       <c r="Y346" s="11"/>
     </row>
-    <row r="347" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B347" s="12">
         <v>44751</v>
       </c>
@@ -10740,7 +11152,7 @@
       <c r="X347" s="15"/>
       <c r="Y347" s="15"/>
     </row>
-    <row r="348" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B348" s="12">
         <v>44752</v>
       </c>
@@ -10768,7 +11180,10 @@
       <c r="X348" s="15"/>
       <c r="Y348" s="15"/>
     </row>
-    <row r="349" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>50</v>
+      </c>
       <c r="B349" s="8">
         <v>44753</v>
       </c>
@@ -10796,7 +11211,7 @@
       <c r="X349" s="11"/>
       <c r="Y349" s="11"/>
     </row>
-    <row r="350" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B350" s="8">
         <v>44754</v>
       </c>
@@ -10824,7 +11239,7 @@
       <c r="X350" s="11"/>
       <c r="Y350" s="11"/>
     </row>
-    <row r="351" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B351" s="8">
         <v>44755</v>
       </c>
@@ -10852,7 +11267,7 @@
       <c r="X351" s="11"/>
       <c r="Y351" s="11"/>
     </row>
-    <row r="352" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B352" s="8">
         <v>44756</v>
       </c>
@@ -10880,7 +11295,7 @@
       <c r="X352" s="11"/>
       <c r="Y352" s="11"/>
     </row>
-    <row r="353" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B353" s="8">
         <v>44757</v>
       </c>
@@ -10908,7 +11323,7 @@
       <c r="X353" s="11"/>
       <c r="Y353" s="11"/>
     </row>
-    <row r="354" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B354" s="12">
         <v>44758</v>
       </c>
@@ -10936,7 +11351,7 @@
       <c r="X354" s="15"/>
       <c r="Y354" s="15"/>
     </row>
-    <row r="355" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B355" s="12">
         <v>44759</v>
       </c>
@@ -10964,7 +11379,10 @@
       <c r="X355" s="15"/>
       <c r="Y355" s="15"/>
     </row>
-    <row r="356" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>51</v>
+      </c>
       <c r="B356" s="8">
         <v>44760</v>
       </c>
@@ -10992,7 +11410,7 @@
       <c r="X356" s="11"/>
       <c r="Y356" s="11"/>
     </row>
-    <row r="357" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B357" s="8">
         <v>44761</v>
       </c>
@@ -11020,7 +11438,7 @@
       <c r="X357" s="11"/>
       <c r="Y357" s="11"/>
     </row>
-    <row r="358" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B358" s="8">
         <v>44762</v>
       </c>
@@ -11048,7 +11466,7 @@
       <c r="X358" s="11"/>
       <c r="Y358" s="11"/>
     </row>
-    <row r="359" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B359" s="8">
         <v>44763</v>
       </c>
@@ -11076,7 +11494,7 @@
       <c r="X359" s="11"/>
       <c r="Y359" s="11"/>
     </row>
-    <row r="360" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B360" s="8">
         <v>44764</v>
       </c>
@@ -11104,7 +11522,7 @@
       <c r="X360" s="11"/>
       <c r="Y360" s="11"/>
     </row>
-    <row r="361" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B361" s="12">
         <v>44765</v>
       </c>
@@ -11132,7 +11550,7 @@
       <c r="X361" s="15"/>
       <c r="Y361" s="15"/>
     </row>
-    <row r="362" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B362" s="12">
         <v>44766</v>
       </c>
@@ -11160,7 +11578,10 @@
       <c r="X362" s="15"/>
       <c r="Y362" s="15"/>
     </row>
-    <row r="363" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A363">
+        <v>52</v>
+      </c>
       <c r="B363" s="8">
         <v>44767</v>
       </c>
@@ -11188,7 +11609,7 @@
       <c r="X363" s="11"/>
       <c r="Y363" s="11"/>
     </row>
-    <row r="364" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B364" s="8">
         <v>44768</v>
       </c>
@@ -11216,7 +11637,7 @@
       <c r="X364" s="11"/>
       <c r="Y364" s="11"/>
     </row>
-    <row r="365" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B365" s="8">
         <v>44769</v>
       </c>
@@ -11244,7 +11665,7 @@
       <c r="X365" s="11"/>
       <c r="Y365" s="11"/>
     </row>
-    <row r="366" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B366" s="8">
         <v>44770</v>
       </c>
@@ -11272,7 +11693,7 @@
       <c r="X366" s="11"/>
       <c r="Y366" s="11"/>
     </row>
-    <row r="367" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B367" s="8">
         <v>44771</v>
       </c>
@@ -11300,7 +11721,7 @@
       <c r="X367" s="11"/>
       <c r="Y367" s="11"/>
     </row>
-    <row r="368" spans="2:25" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B368" s="12">
         <v>44772</v>
       </c>

</xml_diff>